<commit_message>
Bug: Illegal sheet symbols; incomplete cell squares
Close #11.
</commit_message>
<xml_diff>
--- a/assets/basic.xlsx
+++ b/assets/basic.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/User/coding/excel/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\nate\coding\excel\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D6526D18-9887-CD4B-9CF7-C89C5A4BE8A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE4B1C9-873A-43AE-8C5F-6383EE3A5C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16220" xr2:uid="{F5BE8F47-E6D0-F842-8808-7027C9E1441B}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14716" activeTab="1" xr2:uid="{F5BE8F47-E6D0-F842-8808-7027C9E1441B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029" iterate="1" iterateCount="500"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +28,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -393,13 +395,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C93F5B8-EFFB-104A-ADFB-6BC7A6950683}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -407,7 +409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -416,7 +418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -426,7 +428,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A4">
         <f t="shared" ref="A4:A11" si="0">A3+1</f>
         <v>3</v>
@@ -436,7 +438,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -446,7 +448,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -456,7 +458,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -466,7 +468,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -476,7 +478,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -486,7 +488,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -496,13 +498,34 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11">
         <f>SUM($A$2:A11)</f>
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{316707CA-EE9B-44E2-96B5-B257576531B5}">
+  <dimension ref="B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B2">
+        <f>SUM(Sheet1!A2:A11)</f>
         <v>55</v>
       </c>
     </row>

</xml_diff>